<commit_message>
xslx had a space :(
</commit_message>
<xml_diff>
--- a/sources/data.xlsx
+++ b/sources/data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patricia\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D478FC2-A9E6-4CAB-889D-20D5691A7DB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69A67518-DAF3-4506-A5F3-151359E7EF8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2200" yWindow="2200" windowWidth="14400" windowHeight="8180" xr2:uid="{F12530EB-6131-4FCB-A65B-DE99E738297D}"/>
   </bookViews>
@@ -41,9 +41,6 @@
     <t>Alba</t>
   </si>
   <si>
-    <t xml:space="preserve">County </t>
-  </si>
-  <si>
     <t>Arad</t>
   </si>
   <si>
@@ -125,9 +122,6 @@
     <t>Mures</t>
   </si>
   <si>
-    <t>Neamtt</t>
-  </si>
-  <si>
     <t>Olt</t>
   </si>
   <si>
@@ -174,6 +168,12 @@
   </si>
   <si>
     <t>misc</t>
+  </si>
+  <si>
+    <t>County</t>
+  </si>
+  <si>
+    <t>Neamt</t>
   </si>
 </sst>
 </file>
@@ -548,9 +548,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BEC4277-A0E3-4C73-BCC9-DA238430101C}">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
@@ -559,19 +557,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" t="s">
         <v>43</v>
-      </c>
-      <c r="D1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.5">
@@ -593,7 +591,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -610,7 +608,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -627,7 +625,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -644,7 +642,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -661,7 +659,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -678,7 +676,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>2</v>
@@ -695,7 +693,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>2</v>
@@ -712,7 +710,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -729,7 +727,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -746,7 +744,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -763,7 +761,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -780,7 +778,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>2</v>
@@ -797,7 +795,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -814,7 +812,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>2</v>
@@ -831,7 +829,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>2</v>
@@ -848,7 +846,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -865,7 +863,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>2</v>
@@ -882,7 +880,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>2</v>
@@ -899,7 +897,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
         <v>2</v>
@@ -916,7 +914,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
         <v>2</v>
@@ -933,7 +931,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -950,7 +948,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
         <v>2</v>
@@ -967,7 +965,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -984,7 +982,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26">
         <v>2</v>
@@ -1001,7 +999,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27">
         <v>2</v>
@@ -1018,7 +1016,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28">
         <v>2</v>
@@ -1035,7 +1033,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29">
         <v>2</v>
@@ -1052,7 +1050,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="B30">
         <v>2</v>
@@ -1069,7 +1067,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B31">
         <v>2</v>
@@ -1086,7 +1084,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B32">
         <v>2</v>
@@ -1103,7 +1101,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B33">
         <v>2</v>
@@ -1120,7 +1118,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B34">
         <v>2</v>
@@ -1137,7 +1135,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B35">
         <v>2</v>
@@ -1154,7 +1152,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A36" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B36">
         <v>2</v>
@@ -1171,7 +1169,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A37" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B37">
         <v>2</v>
@@ -1188,7 +1186,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B38">
         <v>2</v>
@@ -1205,7 +1203,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A39" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B39">
         <v>2</v>
@@ -1222,7 +1220,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A40" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B40">
         <v>2</v>
@@ -1239,7 +1237,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A41" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B41">
         <v>2</v>
@@ -1256,7 +1254,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A42" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B42">
         <v>2</v>

</xml_diff>